<commit_message>
Listenpreis (Einkaufspreis) zu Aufträgen hinzugefügt
- Neue Spalte: Einkaufspreis (CHF)
- Zeigt den Einkaufspreis netto pro Auftrag
- Ermöglicht Margenberechnung (Verkaufspreis - Einkaufspreis)
</commit_message>
<xml_diff>
--- a/data/Kunden_Auftraege.xlsx
+++ b/data/Kunden_Auftraege.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,8 +477,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -580,20 +581,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -610,12 +616,15 @@
       <c r="D12" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="E12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="G12" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -630,12 +639,15 @@
       <c r="D13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
+      <c r="E13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="G13" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -650,12 +662,15 @@
       <c r="D14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="4" t="inlineStr">
+      <c r="E14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="G14" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -670,12 +685,15 @@
       <c r="D15" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="4" t="inlineStr">
+      <c r="E15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="G15" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -690,12 +708,15 @@
       <c r="D16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E16" s="4" t="inlineStr">
+      <c r="E16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="G16" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -705,17 +726,20 @@
       </c>
       <c r="B17" s="4" t="inlineStr"/>
       <c r="C17" s="5" t="n">
+        <v>8.960000000000001</v>
+      </c>
+      <c r="D17" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="E17" s="5" t="n">
         <v>14.05</v>
       </c>
-      <c r="E17" s="4" t="inlineStr">
+      <c r="F17" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="G17" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -725,17 +749,20 @@
       </c>
       <c r="B18" s="4" t="inlineStr"/>
       <c r="C18" s="5" t="n">
+        <v>184.84</v>
+      </c>
+      <c r="D18" s="5" t="n">
         <v>207.58</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="E18" s="5" t="n">
         <v>224.39</v>
       </c>
-      <c r="E18" s="4" t="inlineStr">
+      <c r="F18" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="G18" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -750,12 +777,15 @@
       <c r="D19" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E19" s="4" t="inlineStr">
+      <c r="E19" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4" t="inlineStr">
         <is>
           <t>Status 25</t>
         </is>
       </c>
-      <c r="F19" s="4" t="n">
+      <c r="G19" s="4" t="n">
         <v>25</v>
       </c>
     </row>
@@ -769,17 +799,20 @@
         </is>
       </c>
       <c r="C20" s="5" t="n">
+        <v>158.97</v>
+      </c>
+      <c r="D20" s="5" t="n">
         <v>166.92</v>
       </c>
-      <c r="D20" s="5" t="n">
+      <c r="E20" s="5" t="n">
         <v>180.44</v>
       </c>
-      <c r="E20" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -793,17 +826,20 @@
         </is>
       </c>
       <c r="C21" s="5" t="n">
+        <v>168.07</v>
+      </c>
+      <c r="D21" s="5" t="n">
         <v>176.92</v>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="E21" s="5" t="n">
         <v>191.25</v>
       </c>
-      <c r="E21" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F21" s="4" t="n">
+      <c r="F21" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -817,17 +853,20 @@
         </is>
       </c>
       <c r="C22" s="5" t="n">
+        <v>166.7</v>
+      </c>
+      <c r="D22" s="5" t="n">
         <v>175.48</v>
       </c>
-      <c r="D22" s="5" t="n">
+      <c r="E22" s="5" t="n">
         <v>189.69</v>
       </c>
-      <c r="E22" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -841,17 +880,20 @@
         </is>
       </c>
       <c r="C23" s="5" t="n">
+        <v>23.88</v>
+      </c>
+      <c r="D23" s="5" t="n">
         <v>25.14</v>
       </c>
-      <c r="D23" s="5" t="n">
+      <c r="E23" s="5" t="n">
         <v>27.18</v>
       </c>
-      <c r="E23" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F23" s="4" t="n">
+      <c r="F23" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -865,17 +907,20 @@
         </is>
       </c>
       <c r="C24" s="5" t="n">
+        <v>96.78</v>
+      </c>
+      <c r="D24" s="5" t="n">
         <v>101.87</v>
       </c>
-      <c r="D24" s="5" t="n">
+      <c r="E24" s="5" t="n">
         <v>110.12</v>
       </c>
-      <c r="E24" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -889,17 +934,20 @@
         </is>
       </c>
       <c r="C25" s="5" t="n">
+        <v>70.06999999999999</v>
+      </c>
+      <c r="D25" s="5" t="n">
         <v>73.76000000000001</v>
       </c>
-      <c r="D25" s="5" t="n">
+      <c r="E25" s="5" t="n">
         <v>79.73</v>
       </c>
-      <c r="E25" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F25" s="4" t="n">
+      <c r="F25" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -913,17 +961,20 @@
         </is>
       </c>
       <c r="C26" s="5" t="n">
+        <v>12.29</v>
+      </c>
+      <c r="D26" s="5" t="n">
         <v>12.94</v>
       </c>
-      <c r="D26" s="5" t="n">
+      <c r="E26" s="5" t="n">
         <v>13.99</v>
       </c>
-      <c r="E26" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -937,17 +988,20 @@
         </is>
       </c>
       <c r="C27" s="5" t="n">
+        <v>135.92</v>
+      </c>
+      <c r="D27" s="5" t="n">
         <v>153.09</v>
       </c>
-      <c r="D27" s="5" t="n">
+      <c r="E27" s="5" t="n">
         <v>165.49</v>
       </c>
-      <c r="E27" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G27" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -961,17 +1015,20 @@
         </is>
       </c>
       <c r="C28" s="5" t="n">
+        <v>1496.86</v>
+      </c>
+      <c r="D28" s="5" t="n">
         <v>1847.94</v>
       </c>
-      <c r="D28" s="5" t="n">
+      <c r="E28" s="5" t="n">
         <v>1997.62</v>
       </c>
-      <c r="E28" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F28" s="4" t="n">
+      <c r="F28" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G28" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -985,17 +1042,20 @@
         </is>
       </c>
       <c r="C29" s="5" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="D29" s="5" t="n">
         <v>25.48</v>
       </c>
-      <c r="D29" s="5" t="n">
+      <c r="E29" s="5" t="n">
         <v>27.54</v>
       </c>
-      <c r="E29" s="4" t="inlineStr">
+      <c r="F29" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F29" s="4" t="n">
+      <c r="G29" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1009,17 +1069,20 @@
         </is>
       </c>
       <c r="C30" s="5" t="n">
+        <v>134.31</v>
+      </c>
+      <c r="D30" s="5" t="n">
         <v>167.89</v>
       </c>
-      <c r="D30" s="5" t="n">
+      <c r="E30" s="5" t="n">
         <v>181.49</v>
       </c>
-      <c r="E30" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F30" s="4" t="n">
+      <c r="F30" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G30" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1033,17 +1096,20 @@
         </is>
       </c>
       <c r="C31" s="5" t="n">
+        <v>68.87</v>
+      </c>
+      <c r="D31" s="5" t="n">
         <v>72.48999999999999</v>
       </c>
-      <c r="D31" s="5" t="n">
+      <c r="E31" s="5" t="n">
         <v>78.36</v>
       </c>
-      <c r="E31" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F31" s="4" t="n">
+      <c r="F31" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1057,17 +1123,20 @@
         </is>
       </c>
       <c r="C32" s="5" t="n">
+        <v>183.15</v>
+      </c>
+      <c r="D32" s="5" t="n">
         <v>191.84</v>
       </c>
-      <c r="D32" s="5" t="n">
+      <c r="E32" s="5" t="n">
         <v>207.38</v>
       </c>
-      <c r="E32" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F32" s="4" t="n">
+      <c r="F32" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G32" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1081,17 +1150,20 @@
         </is>
       </c>
       <c r="C33" s="5" t="n">
+        <v>333.66</v>
+      </c>
+      <c r="D33" s="5" t="n">
         <v>351.24</v>
       </c>
-      <c r="D33" s="5" t="n">
+      <c r="E33" s="5" t="n">
         <v>379.69</v>
       </c>
-      <c r="E33" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F33" s="4" t="n">
+      <c r="F33" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G33" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1105,17 +1177,20 @@
         </is>
       </c>
       <c r="C34" s="5" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="D34" s="5" t="n">
         <v>19.6</v>
       </c>
-      <c r="D34" s="5" t="n">
+      <c r="E34" s="5" t="n">
         <v>21.19</v>
       </c>
-      <c r="E34" s="4" t="inlineStr">
+      <c r="F34" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F34" s="4" t="n">
+      <c r="G34" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1129,17 +1204,20 @@
         </is>
       </c>
       <c r="C35" s="5" t="n">
+        <v>49.84</v>
+      </c>
+      <c r="D35" s="5" t="n">
         <v>63.29</v>
       </c>
-      <c r="D35" s="5" t="n">
+      <c r="E35" s="5" t="n">
         <v>68.42</v>
       </c>
-      <c r="E35" s="4" t="inlineStr">
+      <c r="F35" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F35" s="4" t="n">
+      <c r="G35" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1153,17 +1231,20 @@
         </is>
       </c>
       <c r="C36" s="5" t="n">
+        <v>16.12</v>
+      </c>
+      <c r="D36" s="5" t="n">
         <v>22.57</v>
       </c>
-      <c r="D36" s="5" t="n">
+      <c r="E36" s="5" t="n">
         <v>24.4</v>
       </c>
-      <c r="E36" s="4" t="inlineStr">
+      <c r="F36" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F36" s="4" t="n">
+      <c r="G36" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1177,17 +1258,20 @@
         </is>
       </c>
       <c r="C37" s="5" t="n">
+        <v>88.02</v>
+      </c>
+      <c r="D37" s="5" t="n">
         <v>132.04</v>
       </c>
-      <c r="D37" s="5" t="n">
+      <c r="E37" s="5" t="n">
         <v>142.74</v>
       </c>
-      <c r="E37" s="4" t="inlineStr">
+      <c r="F37" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F37" s="4" t="n">
+      <c r="G37" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1206,12 +1290,15 @@
       <c r="D38" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E38" s="4" t="inlineStr">
+      <c r="E38" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F38" s="4" t="n">
+      <c r="G38" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1225,17 +1312,20 @@
         </is>
       </c>
       <c r="C39" s="5" t="n">
+        <v>24.46</v>
+      </c>
+      <c r="D39" s="5" t="n">
         <v>36.71</v>
       </c>
-      <c r="D39" s="5" t="n">
+      <c r="E39" s="5" t="n">
         <v>39.68</v>
       </c>
-      <c r="E39" s="4" t="inlineStr">
+      <c r="F39" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F39" s="4" t="n">
+      <c r="G39" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1254,12 +1344,15 @@
       <c r="D40" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E40" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F40" s="4" t="n">
+      <c r="E40" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G40" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1278,12 +1371,15 @@
       <c r="D41" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E41" s="4" t="inlineStr">
+      <c r="E41" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F41" s="4" t="n">
+      <c r="G41" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1297,17 +1393,20 @@
         </is>
       </c>
       <c r="C42" s="5" t="n">
+        <v>14.96</v>
+      </c>
+      <c r="D42" s="5" t="n">
         <v>26.92</v>
       </c>
-      <c r="D42" s="5" t="n">
+      <c r="E42" s="5" t="n">
         <v>29.1</v>
       </c>
-      <c r="E42" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F42" s="4" t="n">
+      <c r="F42" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G42" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1321,17 +1420,20 @@
         </is>
       </c>
       <c r="C43" s="5" t="n">
+        <v>16.96</v>
+      </c>
+      <c r="D43" s="5" t="n">
         <v>18.76</v>
       </c>
-      <c r="D43" s="5" t="n">
+      <c r="E43" s="5" t="n">
         <v>20.28</v>
       </c>
-      <c r="E43" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F43" s="4" t="n">
+      <c r="F43" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G43" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1345,17 +1447,20 @@
         </is>
       </c>
       <c r="C44" s="5" t="n">
+        <v>160.47</v>
+      </c>
+      <c r="D44" s="5" t="n">
         <v>200.59</v>
       </c>
-      <c r="D44" s="5" t="n">
+      <c r="E44" s="5" t="n">
         <v>216.84</v>
       </c>
-      <c r="E44" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F44" s="4" t="n">
+      <c r="F44" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G44" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1369,17 +1474,20 @@
         </is>
       </c>
       <c r="C45" s="5" t="n">
+        <v>121.99</v>
+      </c>
+      <c r="D45" s="5" t="n">
         <v>137.3</v>
       </c>
-      <c r="D45" s="5" t="n">
+      <c r="E45" s="5" t="n">
         <v>148.42</v>
       </c>
-      <c r="E45" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F45" s="4" t="n">
+      <c r="F45" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G45" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1393,17 +1501,20 @@
         </is>
       </c>
       <c r="C46" s="5" t="n">
+        <v>217.13</v>
+      </c>
+      <c r="D46" s="5" t="n">
         <v>241.26</v>
       </c>
-      <c r="D46" s="5" t="n">
+      <c r="E46" s="5" t="n">
         <v>260.8</v>
       </c>
-      <c r="E46" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F46" s="4" t="n">
+      <c r="F46" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G46" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -1417,24 +1528,27 @@
         </is>
       </c>
       <c r="C47" s="5" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="D47" s="5" t="n">
         <v>10.78</v>
       </c>
-      <c r="D47" s="5" t="n">
+      <c r="E47" s="5" t="n">
         <v>11.65</v>
       </c>
-      <c r="E47" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F47" s="4" t="n">
+      <c r="F47" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G47" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1446,7 +1560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1458,8 +1572,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -1557,20 +1672,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -1582,24 +1702,27 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>23.49</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>70</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>75.67</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="F12" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="G12" s="4" t="n">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1611,7 +1734,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1623,8 +1746,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -1722,20 +1846,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -1747,24 +1876,27 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>5.34</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>19.6</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>21.19</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="F12" s="4" t="inlineStr">
         <is>
           <t>Status 25</t>
         </is>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="G12" s="4" t="n">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1776,7 +1908,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1788,8 +1920,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -1887,20 +2020,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -1912,24 +2050,27 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>8.06</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>14.39</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>15.56</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="F12" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="G12" s="4" t="n">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1941,7 +2082,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1953,8 +2094,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -2056,20 +2198,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -2081,24 +2228,27 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>136.29</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>198.85</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>214.96</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="F12" s="4" t="inlineStr">
         <is>
           <t>Status 25</t>
         </is>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="G12" s="4" t="n">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2110,7 +2260,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2122,8 +2272,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -2225,20 +2376,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -2250,17 +2406,20 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>1139.85</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>1567.35</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>1694.31</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="F12" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="G12" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2275,12 +2434,15 @@
       <c r="D13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
+      <c r="E13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="G13" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -2294,17 +2456,20 @@
         </is>
       </c>
       <c r="C14" s="5" t="n">
+        <v>93.2</v>
+      </c>
+      <c r="D14" s="5" t="n">
         <v>120</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="E14" s="5" t="n">
         <v>129.72</v>
       </c>
-      <c r="E14" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2318,17 +2483,20 @@
         </is>
       </c>
       <c r="C15" s="5" t="n">
+        <v>87.69</v>
+      </c>
+      <c r="D15" s="5" t="n">
         <v>150.3</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="E15" s="5" t="n">
         <v>162.47</v>
       </c>
-      <c r="E15" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2347,19 +2515,22 @@
       <c r="D16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E16" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F16" s="4" t="n">
+      <c r="E16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2371,7 +2542,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2383,8 +2554,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -2482,20 +2654,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -2507,17 +2684,20 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>8169.45</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>10688.85</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>11554.65</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2527,24 +2707,27 @@
       </c>
       <c r="B13" s="4" t="inlineStr"/>
       <c r="C13" s="5" t="n">
+        <v>2021.55</v>
+      </c>
+      <c r="D13" s="5" t="n">
         <v>3470.85</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="E13" s="5" t="n">
         <v>3751.99</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2556,7 +2739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2568,8 +2751,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -2675,20 +2859,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -2704,24 +2893,27 @@
         </is>
       </c>
       <c r="C12" s="5" t="n">
+        <v>54.77</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>103.11</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>111.46</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2733,7 +2925,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2745,8 +2937,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -2852,20 +3045,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -2877,17 +3075,20 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>28.39</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>51.79</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>55.98</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2897,17 +3098,20 @@
       </c>
       <c r="B13" s="4" t="inlineStr"/>
       <c r="C13" s="5" t="n">
+        <v>72.48999999999999</v>
+      </c>
+      <c r="D13" s="5" t="n">
         <v>110.01</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="E13" s="5" t="n">
         <v>118.92</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2921,17 +3125,20 @@
         </is>
       </c>
       <c r="C14" s="5" t="n">
+        <v>130.88</v>
+      </c>
+      <c r="D14" s="5" t="n">
         <v>169</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="E14" s="5" t="n">
         <v>182.69</v>
       </c>
-      <c r="E14" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -2945,24 +3152,27 @@
         </is>
       </c>
       <c r="C15" s="5" t="n">
+        <v>73.90000000000001</v>
+      </c>
+      <c r="D15" s="5" t="n">
         <v>129.31</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="E15" s="5" t="n">
         <v>139.78</v>
       </c>
-      <c r="E15" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2974,7 +3184,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2986,8 +3196,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -3093,20 +3304,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -3118,17 +3334,20 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>24.45</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>91.12</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>98.5</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3138,17 +3357,20 @@
       </c>
       <c r="B13" s="4" t="inlineStr"/>
       <c r="C13" s="5" t="n">
+        <v>920.96</v>
+      </c>
+      <c r="D13" s="5" t="n">
         <v>1251.04</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="E13" s="5" t="n">
         <v>1352.37</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3163,12 +3385,15 @@
       <c r="D14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="4" t="inlineStr">
+      <c r="E14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4" t="inlineStr">
         <is>
           <t>Status 25</t>
         </is>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="G14" s="4" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3187,12 +3412,15 @@
       <c r="D15" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F15" s="4" t="n">
+      <c r="E15" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3206,17 +3434,20 @@
         </is>
       </c>
       <c r="C16" s="5" t="n">
+        <v>188.81</v>
+      </c>
+      <c r="D16" s="5" t="n">
         <v>609.0700000000001</v>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="E16" s="5" t="n">
         <v>658.4</v>
       </c>
-      <c r="E16" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3235,12 +3466,15 @@
       <c r="D17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E17" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F17" s="4" t="n">
+      <c r="E17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3259,12 +3493,15 @@
       <c r="D18" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E18" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F18" s="4" t="n">
+      <c r="E18" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3278,17 +3515,20 @@
         </is>
       </c>
       <c r="C19" s="5" t="n">
+        <v>475.05</v>
+      </c>
+      <c r="D19" s="5" t="n">
         <v>793.08</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="E19" s="5" t="n">
         <v>857.3200000000001</v>
       </c>
-      <c r="E19" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F19" s="4" t="n">
+      <c r="F19" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3302,17 +3542,20 @@
         </is>
       </c>
       <c r="C20" s="5" t="n">
+        <v>11.43</v>
+      </c>
+      <c r="D20" s="5" t="n">
         <v>39.63</v>
       </c>
-      <c r="D20" s="5" t="n">
+      <c r="E20" s="5" t="n">
         <v>42.84</v>
       </c>
-      <c r="E20" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3326,17 +3569,20 @@
         </is>
       </c>
       <c r="C21" s="5" t="n">
+        <v>299.52</v>
+      </c>
+      <c r="D21" s="5" t="n">
         <v>622.52</v>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="E21" s="5" t="n">
         <v>672.9400000000001</v>
       </c>
-      <c r="E21" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F21" s="4" t="n">
+      <c r="F21" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3350,17 +3596,20 @@
         </is>
       </c>
       <c r="C22" s="5" t="n">
+        <v>44.43</v>
+      </c>
+      <c r="D22" s="5" t="n">
         <v>125.5</v>
       </c>
-      <c r="D22" s="5" t="n">
+      <c r="E22" s="5" t="n">
         <v>135.67</v>
       </c>
-      <c r="E22" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3374,17 +3623,20 @@
         </is>
       </c>
       <c r="C23" s="5" t="n">
+        <v>318.2</v>
+      </c>
+      <c r="D23" s="5" t="n">
         <v>622.51</v>
       </c>
-      <c r="D23" s="5" t="n">
+      <c r="E23" s="5" t="n">
         <v>672.9299999999999</v>
       </c>
-      <c r="E23" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F23" s="4" t="n">
+      <c r="F23" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3398,17 +3650,20 @@
         </is>
       </c>
       <c r="C24" s="5" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="D24" s="5" t="n">
         <v>73</v>
       </c>
-      <c r="D24" s="5" t="n">
+      <c r="E24" s="5" t="n">
         <v>78.91</v>
       </c>
-      <c r="E24" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3422,17 +3677,20 @@
         </is>
       </c>
       <c r="C25" s="5" t="n">
+        <v>107.51</v>
+      </c>
+      <c r="D25" s="5" t="n">
         <v>202.46</v>
       </c>
-      <c r="D25" s="5" t="n">
+      <c r="E25" s="5" t="n">
         <v>218.86</v>
       </c>
-      <c r="E25" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F25" s="4" t="n">
+      <c r="F25" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3446,17 +3704,20 @@
         </is>
       </c>
       <c r="C26" s="5" t="n">
+        <v>81.76000000000001</v>
+      </c>
+      <c r="D26" s="5" t="n">
         <v>189.3</v>
       </c>
-      <c r="D26" s="5" t="n">
+      <c r="E26" s="5" t="n">
         <v>204.63</v>
       </c>
-      <c r="E26" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3470,17 +3731,20 @@
         </is>
       </c>
       <c r="C27" s="5" t="n">
+        <v>24.19</v>
+      </c>
+      <c r="D27" s="5" t="n">
         <v>110</v>
       </c>
-      <c r="D27" s="5" t="n">
+      <c r="E27" s="5" t="n">
         <v>118.91</v>
       </c>
-      <c r="E27" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G27" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3494,17 +3758,20 @@
         </is>
       </c>
       <c r="C28" s="5" t="n">
+        <v>159.71</v>
+      </c>
+      <c r="D28" s="5" t="n">
         <v>362.69</v>
       </c>
-      <c r="D28" s="5" t="n">
+      <c r="E28" s="5" t="n">
         <v>392.07</v>
       </c>
-      <c r="E28" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F28" s="4" t="n">
+      <c r="F28" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G28" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3518,17 +3785,20 @@
         </is>
       </c>
       <c r="C29" s="5" t="n">
+        <v>24.19</v>
+      </c>
+      <c r="D29" s="5" t="n">
         <v>75</v>
       </c>
-      <c r="D29" s="5" t="n">
+      <c r="E29" s="5" t="n">
         <v>81.08</v>
       </c>
-      <c r="E29" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F29" s="4" t="n">
+      <c r="F29" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G29" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3542,17 +3812,20 @@
         </is>
       </c>
       <c r="C30" s="5" t="n">
+        <v>61.59</v>
+      </c>
+      <c r="D30" s="5" t="n">
         <v>260.54</v>
       </c>
-      <c r="D30" s="5" t="n">
+      <c r="E30" s="5" t="n">
         <v>281.64</v>
       </c>
-      <c r="E30" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F30" s="4" t="n">
+      <c r="F30" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G30" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3566,17 +3839,20 @@
         </is>
       </c>
       <c r="C31" s="5" t="n">
+        <v>124.51</v>
+      </c>
+      <c r="D31" s="5" t="n">
         <v>200.23</v>
       </c>
-      <c r="D31" s="5" t="n">
+      <c r="E31" s="5" t="n">
         <v>216.45</v>
       </c>
-      <c r="E31" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F31" s="4" t="n">
+      <c r="F31" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3590,17 +3866,20 @@
         </is>
       </c>
       <c r="C32" s="5" t="n">
+        <v>48.16</v>
+      </c>
+      <c r="D32" s="5" t="n">
         <v>193.73</v>
       </c>
-      <c r="D32" s="5" t="n">
+      <c r="E32" s="5" t="n">
         <v>209.42</v>
       </c>
-      <c r="E32" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F32" s="4" t="n">
+      <c r="F32" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G32" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3614,24 +3893,27 @@
         </is>
       </c>
       <c r="C33" s="5" t="n">
+        <v>70.92</v>
+      </c>
+      <c r="D33" s="5" t="n">
         <v>120.54</v>
       </c>
-      <c r="D33" s="5" t="n">
+      <c r="E33" s="5" t="n">
         <v>130.3</v>
       </c>
-      <c r="E33" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F33" s="4" t="n">
+      <c r="F33" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G33" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3643,7 +3925,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3655,8 +3937,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -3758,20 +4041,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -3783,17 +4071,20 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>947.92</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>3202.76</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>3462.18</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="F12" s="4" t="inlineStr">
         <is>
           <t>Status 25</t>
         </is>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="G12" s="4" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3803,17 +4094,20 @@
       </c>
       <c r="B13" s="4" t="inlineStr"/>
       <c r="C13" s="5" t="n">
+        <v>475.1</v>
+      </c>
+      <c r="D13" s="5" t="n">
         <v>1534.23</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="E13" s="5" t="n">
         <v>1658.5</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
+      <c r="F13" s="4" t="inlineStr">
         <is>
           <t>Status 25</t>
         </is>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="G13" s="4" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3823,17 +4117,20 @@
       </c>
       <c r="B14" s="4" t="inlineStr"/>
       <c r="C14" s="5" t="n">
+        <v>12038</v>
+      </c>
+      <c r="D14" s="5" t="n">
         <v>15400</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="E14" s="5" t="n">
         <v>16647.4</v>
       </c>
-      <c r="E14" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3847,17 +4144,20 @@
         </is>
       </c>
       <c r="C15" s="5" t="n">
+        <v>367.92</v>
+      </c>
+      <c r="D15" s="5" t="n">
         <v>510</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="E15" s="5" t="n">
         <v>551.3099999999999</v>
       </c>
-      <c r="E15" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3871,17 +4171,20 @@
         </is>
       </c>
       <c r="C16" s="5" t="n">
+        <v>1185.8</v>
+      </c>
+      <c r="D16" s="5" t="n">
         <v>1160</v>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="E16" s="5" t="n">
         <v>1253.96</v>
       </c>
-      <c r="E16" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3895,17 +4198,20 @@
         </is>
       </c>
       <c r="C17" s="5" t="n">
+        <v>1067.26</v>
+      </c>
+      <c r="D17" s="5" t="n">
         <v>1637.92</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="E17" s="5" t="n">
         <v>1770.59</v>
       </c>
-      <c r="E17" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3919,17 +4225,20 @@
         </is>
       </c>
       <c r="C18" s="5" t="n">
+        <v>454.31</v>
+      </c>
+      <c r="D18" s="5" t="n">
         <v>840</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="E18" s="5" t="n">
         <v>908.04</v>
       </c>
-      <c r="E18" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -3943,24 +4252,27 @@
         </is>
       </c>
       <c r="C19" s="5" t="n">
+        <v>208.66</v>
+      </c>
+      <c r="D19" s="5" t="n">
         <v>429.59</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="E19" s="5" t="n">
         <v>464.39</v>
       </c>
-      <c r="E19" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F19" s="4" t="n">
+      <c r="F19" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3972,7 +4284,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3984,8 +4296,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -4083,20 +4396,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -4108,17 +4426,20 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>448.82</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>548.0700000000001</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>592.46</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4133,12 +4454,15 @@
       <c r="D13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
+      <c r="E13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="G13" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -4148,17 +4472,20 @@
       </c>
       <c r="B14" s="4" t="inlineStr"/>
       <c r="C14" s="5" t="n">
+        <v>316.45</v>
+      </c>
+      <c r="D14" s="5" t="n">
         <v>495.02</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="E14" s="5" t="n">
         <v>535.12</v>
       </c>
-      <c r="E14" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4168,17 +4495,20 @@
       </c>
       <c r="B15" s="4" t="inlineStr"/>
       <c r="C15" s="5" t="n">
+        <v>352.28</v>
+      </c>
+      <c r="D15" s="5" t="n">
         <v>439.88</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="E15" s="5" t="n">
         <v>475.51</v>
       </c>
-      <c r="E15" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4188,17 +4518,20 @@
       </c>
       <c r="B16" s="4" t="inlineStr"/>
       <c r="C16" s="5" t="n">
+        <v>130.88</v>
+      </c>
+      <c r="D16" s="5" t="n">
         <v>159</v>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="E16" s="5" t="n">
         <v>171.88</v>
       </c>
-      <c r="E16" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4217,12 +4550,15 @@
       <c r="D17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E17" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F17" s="4" t="n">
+      <c r="E17" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4236,17 +4572,20 @@
         </is>
       </c>
       <c r="C18" s="5" t="n">
+        <v>125.04</v>
+      </c>
+      <c r="D18" s="5" t="n">
         <v>212.44</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="E18" s="5" t="n">
         <v>229.65</v>
       </c>
-      <c r="E18" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4260,17 +4599,20 @@
         </is>
       </c>
       <c r="C19" s="5" t="n">
+        <v>123.6</v>
+      </c>
+      <c r="D19" s="5" t="n">
         <v>185.02</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="E19" s="5" t="n">
         <v>200.01</v>
       </c>
-      <c r="E19" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F19" s="4" t="n">
+      <c r="F19" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4289,19 +4631,22 @@
       <c r="D20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E20" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F20" s="4" t="n">
+      <c r="E20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4313,7 +4658,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4325,8 +4670,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -4428,20 +4774,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -4453,17 +4804,20 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>49.32</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>106.38</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>115</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4477,24 +4831,27 @@
         </is>
       </c>
       <c r="C13" s="5" t="n">
+        <v>31.57</v>
+      </c>
+      <c r="D13" s="5" t="n">
         <v>100.66</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="E13" s="5" t="n">
         <v>108.81</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4506,7 +4863,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4518,8 +4875,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -4617,20 +4975,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -4642,17 +5005,20 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>305.59</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>590.21</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>638.02</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="F12" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="G12" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -4662,17 +5028,20 @@
       </c>
       <c r="B13" s="4" t="inlineStr"/>
       <c r="C13" s="5" t="n">
+        <v>181.47</v>
+      </c>
+      <c r="D13" s="5" t="n">
         <v>284.06</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="E13" s="5" t="n">
         <v>307.07</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4687,12 +5056,15 @@
       <c r="D14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="4" t="inlineStr">
+      <c r="E14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="G14" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -4702,17 +5074,20 @@
       </c>
       <c r="B15" s="4" t="inlineStr"/>
       <c r="C15" s="5" t="n">
+        <v>23.49</v>
+      </c>
+      <c r="D15" s="5" t="n">
         <v>64.68000000000001</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="E15" s="5" t="n">
         <v>69.92</v>
       </c>
-      <c r="E15" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4727,12 +5102,15 @@
       <c r="D16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E16" s="4" t="inlineStr">
+      <c r="E16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="G16" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -4742,17 +5120,20 @@
       </c>
       <c r="B17" s="4" t="inlineStr"/>
       <c r="C17" s="5" t="n">
+        <v>257.28</v>
+      </c>
+      <c r="D17" s="5" t="n">
         <v>326.5</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="E17" s="5" t="n">
         <v>352.95</v>
       </c>
-      <c r="E17" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4762,17 +5143,20 @@
       </c>
       <c r="B18" s="4" t="inlineStr"/>
       <c r="C18" s="5" t="n">
+        <v>128.3</v>
+      </c>
+      <c r="D18" s="5" t="n">
         <v>340.9</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="E18" s="5" t="n">
         <v>368.51</v>
       </c>
-      <c r="E18" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4782,17 +5166,20 @@
       </c>
       <c r="B19" s="4" t="inlineStr"/>
       <c r="C19" s="5" t="n">
+        <v>59.24</v>
+      </c>
+      <c r="D19" s="5" t="n">
         <v>150</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="E19" s="5" t="n">
         <v>162.15</v>
       </c>
-      <c r="E19" s="4" t="inlineStr">
+      <c r="F19" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F19" s="4" t="n">
+      <c r="G19" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -4807,12 +5194,15 @@
       <c r="D20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E20" s="4" t="inlineStr">
+      <c r="E20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="G20" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -4826,17 +5216,20 @@
         </is>
       </c>
       <c r="C21" s="5" t="n">
+        <v>295.34</v>
+      </c>
+      <c r="D21" s="5" t="n">
         <v>263.66</v>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="E21" s="5" t="n">
         <v>285.02</v>
       </c>
-      <c r="E21" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F21" s="4" t="n">
+      <c r="F21" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4850,17 +5243,20 @@
         </is>
       </c>
       <c r="C22" s="5" t="n">
+        <v>140.3</v>
+      </c>
+      <c r="D22" s="5" t="n">
         <v>185.01</v>
       </c>
-      <c r="D22" s="5" t="n">
+      <c r="E22" s="5" t="n">
         <v>200</v>
       </c>
-      <c r="E22" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4874,17 +5270,20 @@
         </is>
       </c>
       <c r="C23" s="5" t="n">
+        <v>60.34</v>
+      </c>
+      <c r="D23" s="5" t="n">
         <v>105</v>
       </c>
-      <c r="D23" s="5" t="n">
+      <c r="E23" s="5" t="n">
         <v>113.51</v>
       </c>
-      <c r="E23" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F23" s="4" t="n">
+      <c r="F23" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4898,17 +5297,20 @@
         </is>
       </c>
       <c r="C24" s="5" t="n">
+        <v>378.43</v>
+      </c>
+      <c r="D24" s="5" t="n">
         <v>630.91</v>
       </c>
-      <c r="D24" s="5" t="n">
+      <c r="E24" s="5" t="n">
         <v>682.01</v>
       </c>
-      <c r="E24" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4922,17 +5324,20 @@
         </is>
       </c>
       <c r="C25" s="5" t="n">
+        <v>86.34</v>
+      </c>
+      <c r="D25" s="5" t="n">
         <v>127.27</v>
       </c>
-      <c r="D25" s="5" t="n">
+      <c r="E25" s="5" t="n">
         <v>137.58</v>
       </c>
-      <c r="E25" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F25" s="4" t="n">
+      <c r="F25" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4946,17 +5351,20 @@
         </is>
       </c>
       <c r="C26" s="5" t="n">
+        <v>87.69</v>
+      </c>
+      <c r="D26" s="5" t="n">
         <v>137.43</v>
       </c>
-      <c r="D26" s="5" t="n">
+      <c r="E26" s="5" t="n">
         <v>148.56</v>
       </c>
-      <c r="E26" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4970,17 +5378,20 @@
         </is>
       </c>
       <c r="C27" s="5" t="n">
+        <v>42.08</v>
+      </c>
+      <c r="D27" s="5" t="n">
         <v>59.67</v>
       </c>
-      <c r="D27" s="5" t="n">
+      <c r="E27" s="5" t="n">
         <v>64.5</v>
       </c>
-      <c r="E27" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G27" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4994,24 +5405,27 @@
         </is>
       </c>
       <c r="C28" s="5" t="n">
+        <v>76.84</v>
+      </c>
+      <c r="D28" s="5" t="n">
         <v>120.01</v>
       </c>
-      <c r="D28" s="5" t="n">
+      <c r="E28" s="5" t="n">
         <v>129.73</v>
       </c>
-      <c r="E28" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F28" s="4" t="n">
+      <c r="F28" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G28" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5023,7 +5437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5035,8 +5449,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -5134,20 +5549,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -5163,24 +5583,27 @@
         </is>
       </c>
       <c r="C12" s="5" t="n">
+        <v>207.24</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>255.38</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>276.07</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5192,7 +5615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5204,8 +5627,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -5307,20 +5731,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -5332,17 +5761,20 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>363.53</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>768.71</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>830.98</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -5357,12 +5789,15 @@
       <c r="D13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
+      <c r="E13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="G13" s="4" t="n">
         <v>27</v>
       </c>
     </row>
@@ -5376,17 +5811,20 @@
         </is>
       </c>
       <c r="C14" s="5" t="n">
+        <v>337.92</v>
+      </c>
+      <c r="D14" s="5" t="n">
         <v>560</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="E14" s="5" t="n">
         <v>605.36</v>
       </c>
-      <c r="E14" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="n">
         <v>26</v>
       </c>
     </row>
@@ -5400,24 +5838,27 @@
         </is>
       </c>
       <c r="C15" s="5" t="n">
+        <v>215.06</v>
+      </c>
+      <c r="D15" s="5" t="n">
         <v>480</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="E15" s="5" t="n">
         <v>518.88</v>
       </c>
-      <c r="E15" s="4" t="inlineStr">
-        <is>
-          <t>Abgeschlossen</t>
-        </is>
-      </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="4" t="inlineStr">
+        <is>
+          <t>Abgeschlossen</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="n">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5429,7 +5870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5441,8 +5882,9 @@
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -5540,20 +5982,25 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
+          <t>Einkaufspreis (CHF)</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
           <t>Betrag Netto (CHF)</t>
         </is>
       </c>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Betrag Brutto (CHF)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>Status-Code</t>
         </is>
@@ -5565,24 +6012,27 @@
       </c>
       <c r="B12" s="4" t="inlineStr"/>
       <c r="C12" s="5" t="n">
+        <v>7.06</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>19.6</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="E12" s="5" t="n">
         <v>21.19</v>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="F12" s="4" t="inlineStr">
         <is>
           <t>Offen</t>
         </is>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="G12" s="4" t="n">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>